<commit_message>
DEV: Edited Bar charts
</commit_message>
<xml_diff>
--- a/reports/presentation_latex_version/data/chap_04_combined_model_coefs_df.xlsx
+++ b/reports/presentation_latex_version/data/chap_04_combined_model_coefs_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="23">
   <si>
     <t>coef</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>chap_07_msm_central_bank_policy_rates_model_b1.txt</t>
+  </si>
+  <si>
+    <t>chap_07_msm_3m_interbank_lending_rates_oil_gas_rol_vol_model_b2.txt</t>
   </si>
   <si>
     <t>Regime 0 parameters</t>
@@ -437,7 +440,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -480,16 +483,16 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>5.473E-06</v>
+        <v>5.809E-06</v>
       </c>
       <c r="C2">
         <v>8.02E-05</v>
       </c>
       <c r="D2">
-        <v>0.068</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="E2">
-        <v>0.946</v>
+        <v>0.9419999999999999</v>
       </c>
       <c r="F2">
         <v>-0</v>
@@ -506,22 +509,22 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>-2.335E-05</v>
+        <v>-2.292E-05</v>
       </c>
       <c r="C3">
         <v>6.1E-05</v>
       </c>
       <c r="D3">
-        <v>-0.383</v>
+        <v>-0.376</v>
       </c>
       <c r="E3">
-        <v>0.702</v>
+        <v>0.707</v>
       </c>
       <c r="F3">
         <v>-0</v>
       </c>
       <c r="G3">
-        <v>9.63E-05</v>
+        <v>9.66E-05</v>
       </c>
       <c r="H3" t="s">
         <v>16</v>
@@ -584,16 +587,16 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>-0.0002</v>
+        <v>0.0003</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>9.75E-05</v>
       </c>
       <c r="E6">
-        <v>0.232</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="F6">
-        <v>-0</v>
+        <v>6.51E-05</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -602,10 +605,10 @@
         <v>18</v>
       </c>
       <c r="I6">
-        <v>-1.195</v>
+        <v>2.628</v>
       </c>
       <c r="J6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -613,28 +616,28 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>-0.0001</v>
+        <v>-0.0002</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>7.330000000000001E-05</v>
       </c>
       <c r="E7">
-        <v>0.8070000000000001</v>
+        <v>0.016</v>
       </c>
       <c r="F7">
-        <v>-0.001</v>
+        <v>-0</v>
       </c>
       <c r="G7">
-        <v>0.001</v>
+        <v>-3.36E-05</v>
       </c>
       <c r="H7" t="s">
         <v>18</v>
       </c>
       <c r="I7">
-        <v>-0.244</v>
+        <v>-2.418</v>
       </c>
       <c r="J7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -642,28 +645,28 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>5.445E-05</v>
+        <v>1.491E-05</v>
       </c>
       <c r="C8">
-        <v>2.01E-06</v>
+        <v>5.43E-07</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>5.05E-05</v>
+        <v>1.38E-05</v>
       </c>
       <c r="G8">
-        <v>5.84E-05</v>
+        <v>1.6E-05</v>
       </c>
       <c r="H8" t="s">
         <v>18</v>
       </c>
       <c r="I8">
-        <v>27.103</v>
+        <v>27.46</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -671,28 +674,28 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>0.0004</v>
+        <v>-0.0001</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0.002</v>
+        <v>0.381</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="G9">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="H9" t="s">
         <v>18</v>
       </c>
       <c r="I9">
-        <v>3.086</v>
+        <v>-0.877</v>
       </c>
       <c r="J9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -700,28 +703,28 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>-0.0009</v>
+        <v>1.645E-05</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>8.890000000000001E-05</v>
       </c>
       <c r="E10">
-        <v>0.004</v>
+        <v>0.853</v>
       </c>
       <c r="F10">
-        <v>-0.002</v>
+        <v>-0</v>
       </c>
       <c r="G10">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H10" t="s">
         <v>18</v>
       </c>
       <c r="I10">
-        <v>-2.854</v>
+        <v>0.185</v>
       </c>
       <c r="J10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -729,28 +732,28 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>1.883E-05</v>
+        <v>5.012E-05</v>
       </c>
       <c r="C11">
-        <v>9.69E-07</v>
+        <v>1.53E-06</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>1.69E-05</v>
+        <v>4.71E-05</v>
       </c>
       <c r="G11">
-        <v>2.07E-05</v>
+        <v>5.31E-05</v>
       </c>
       <c r="H11" t="s">
         <v>18</v>
       </c>
       <c r="I11">
-        <v>19.428</v>
+        <v>32.656</v>
       </c>
       <c r="J11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -758,7 +761,7 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>0.9917</v>
+        <v>0.9897</v>
       </c>
       <c r="C12">
         <v>0.003</v>
@@ -767,19 +770,19 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>0.987</v>
+        <v>0.984</v>
       </c>
       <c r="G12">
-        <v>0.997</v>
+        <v>0.995</v>
       </c>
       <c r="H12" t="s">
         <v>18</v>
       </c>
       <c r="I12">
-        <v>376.659</v>
+        <v>373.08</v>
       </c>
       <c r="J12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -787,28 +790,260 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>0.0095</v>
+        <v>0.0091</v>
       </c>
       <c r="C13">
         <v>0.003</v>
       </c>
       <c r="E13">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>0.004</v>
       </c>
       <c r="G13">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
       <c r="H13" t="s">
         <v>18</v>
       </c>
       <c r="I13">
+        <v>3.568</v>
+      </c>
+      <c r="J13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>-0.0002</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0.232</v>
+      </c>
+      <c r="F14">
+        <v>-0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14">
+        <v>-1.195</v>
+      </c>
+      <c r="J14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>-0.0001</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0.8070000000000001</v>
+      </c>
+      <c r="F15">
+        <v>-0.001</v>
+      </c>
+      <c r="G15">
+        <v>0.001</v>
+      </c>
+      <c r="H15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15">
+        <v>-0.244</v>
+      </c>
+      <c r="J15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>5.445E-05</v>
+      </c>
+      <c r="C16">
+        <v>2.01E-06</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>5.05E-05</v>
+      </c>
+      <c r="G16">
+        <v>5.84E-05</v>
+      </c>
+      <c r="H16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16">
+        <v>27.103</v>
+      </c>
+      <c r="J16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>0.0004</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0.002</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0.001</v>
+      </c>
+      <c r="H17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17">
+        <v>3.086</v>
+      </c>
+      <c r="J17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>-0.0009</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0.004</v>
+      </c>
+      <c r="F18">
+        <v>-0.002</v>
+      </c>
+      <c r="G18">
+        <v>-0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18">
+        <v>-2.854</v>
+      </c>
+      <c r="J18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>1.883E-05</v>
+      </c>
+      <c r="C19">
+        <v>9.69E-07</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1.69E-05</v>
+      </c>
+      <c r="G19">
+        <v>2.07E-05</v>
+      </c>
+      <c r="H19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19">
+        <v>19.428</v>
+      </c>
+      <c r="J19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20">
+        <v>0.9917</v>
+      </c>
+      <c r="C20">
+        <v>0.003</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0.987</v>
+      </c>
+      <c r="G20">
+        <v>0.997</v>
+      </c>
+      <c r="H20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20">
+        <v>376.659</v>
+      </c>
+      <c r="J20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>0.0095</v>
+      </c>
+      <c r="C21">
+        <v>0.003</v>
+      </c>
+      <c r="E21">
+        <v>0.001</v>
+      </c>
+      <c r="F21">
+        <v>0.004</v>
+      </c>
+      <c r="G21">
+        <v>0.015</v>
+      </c>
+      <c r="H21" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21">
         <v>3.198</v>
       </c>
-      <c r="J13" t="s">
-        <v>21</v>
+      <c r="J21" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>